<commit_message>
ajout produit categorie D BD3
</commit_message>
<xml_diff>
--- a/Datasets/DB3.xlsx
+++ b/Datasets/DB3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours M2\S1\Transparence des algorithmes\Projet\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USB 08.04.20\M2\S1\décision\projet\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E5B8569-EB7A-4A40-93D5-E8038055ACB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB75A0C9-A41E-4327-812F-4E0BF02DB29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6EC24849-5032-4A96-8811-E4B54FE51E76}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6EC24849-5032-4A96-8811-E4B54FE51E76}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
   <si>
     <t>code</t>
   </si>
@@ -142,6 +142,120 @@
   </si>
   <si>
     <t>label_bio</t>
+  </si>
+  <si>
+    <t>5413458064879</t>
+  </si>
+  <si>
+    <t>3564700713235</t>
+  </si>
+  <si>
+    <t>3270160202706</t>
+  </si>
+  <si>
+    <t>3261055947093</t>
+  </si>
+  <si>
+    <t>3770009392044</t>
+  </si>
+  <si>
+    <t>3770009392051</t>
+  </si>
+  <si>
+    <t>213311065143</t>
+  </si>
+  <si>
+    <t>2227171006138</t>
+  </si>
+  <si>
+    <t>3760152390691</t>
+  </si>
+  <si>
+    <t>5413458017578</t>
+  </si>
+  <si>
+    <t>213400032605</t>
+  </si>
+  <si>
+    <t>4056489030942</t>
+  </si>
+  <si>
+    <t>Kipfilet filet de poulet</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>5400141319460</t>
+  </si>
+  <si>
+    <t>Emincés de poulet traité en salaison cuite et grillé</t>
+  </si>
+  <si>
+    <t>Processed meat</t>
+  </si>
+  <si>
+    <t>Lamelles de poulet</t>
+  </si>
+  <si>
+    <t>Filet de poulet</t>
+  </si>
+  <si>
+    <t>Lamelles poulet précuites Aldi Delifin</t>
+  </si>
+  <si>
+    <t>Emincés de poulet "J'Aime"</t>
+  </si>
+  <si>
+    <t>Roti de Pollo</t>
+  </si>
+  <si>
+    <t>Knacki 100% poulet</t>
+  </si>
+  <si>
+    <t>Pollo relleno asado al horno</t>
+  </si>
+  <si>
+    <t>Poulet hawaï</t>
+  </si>
+  <si>
+    <t>Salty snacks</t>
+  </si>
+  <si>
+    <t>Salty and fatty products</t>
+  </si>
+  <si>
+    <t>Allumettes de poulet fumées</t>
+  </si>
+  <si>
+    <t>Blanc de poulet</t>
+  </si>
+  <si>
+    <t>3256221978063</t>
+  </si>
+  <si>
+    <t>5400112591703</t>
+  </si>
+  <si>
+    <t>5400141323986</t>
+  </si>
+  <si>
+    <t>3095759136015</t>
+  </si>
+  <si>
+    <t>8437002390228</t>
+  </si>
+  <si>
+    <t>7613035287167</t>
+  </si>
+  <si>
+    <t>8437005669765</t>
+  </si>
+  <si>
+    <t>3512690003393</t>
+  </si>
+  <si>
+    <t>3560071011383</t>
   </si>
 </sst>
 </file>
@@ -177,8 +291,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,19 +608,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B926D4-B8FA-4885-AAED-407EDDBDF88F}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -563,9 +678,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>5413458064879</v>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
@@ -622,9 +737,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>3564700713235</v>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -681,9 +796,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>4056489030942</v>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -740,9 +855,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3270160202706</v>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -799,9 +914,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>213400032605</v>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -858,9 +973,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>5413458017578</v>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -917,9 +1032,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>3261055947093</v>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
@@ -976,9 +1091,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>3760152390691</v>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
@@ -1035,9 +1150,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>3770009392051</v>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B10" t="s">
         <v>29</v>
@@ -1094,9 +1209,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>3770009392044</v>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -1153,9 +1268,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>2227171006138</v>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
@@ -1212,9 +1327,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>213311065143</v>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
@@ -1271,7 +1386,716 @@
         <v>32</v>
       </c>
     </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38">
+        <v>544</v>
+      </c>
+      <c r="I38">
+        <v>1.7</v>
+      </c>
+      <c r="J38">
+        <v>1.2</v>
+      </c>
+      <c r="K38">
+        <v>0.84</v>
+      </c>
+      <c r="L38">
+        <v>17</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>5.6</v>
+      </c>
+      <c r="O38">
+        <v>1.7</v>
+      </c>
+      <c r="P38">
+        <v>1.2</v>
+      </c>
+      <c r="Q38">
+        <v>2.1</v>
+      </c>
+      <c r="R38">
+        <v>9</v>
+      </c>
+      <c r="S38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" t="s">
+        <v>52</v>
+      </c>
+      <c r="H39">
+        <v>728</v>
+      </c>
+      <c r="I39">
+        <v>2.5</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="L39">
+        <v>21</v>
+      </c>
+      <c r="M39">
+        <v>1.5</v>
+      </c>
+      <c r="N39">
+        <v>9</v>
+      </c>
+      <c r="O39">
+        <v>2.5</v>
+      </c>
+      <c r="P39">
+        <v>1</v>
+      </c>
+      <c r="Q39">
+        <v>1.855</v>
+      </c>
+      <c r="R39">
+        <v>33</v>
+      </c>
+      <c r="S39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40">
+        <v>451</v>
+      </c>
+      <c r="I40">
+        <v>1.2000000476837001</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>0.83999996185304004</v>
+      </c>
+      <c r="L40">
+        <v>19</v>
+      </c>
+      <c r="M40">
+        <v>0.1</v>
+      </c>
+      <c r="N40">
+        <v>3</v>
+      </c>
+      <c r="O40">
+        <v>1.2000000476837001</v>
+      </c>
+      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="Q40">
+        <v>2.0999999046325999</v>
+      </c>
+      <c r="R40">
+        <v>9</v>
+      </c>
+      <c r="S40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41">
+        <v>544</v>
+      </c>
+      <c r="I41">
+        <v>1.7</v>
+      </c>
+      <c r="J41">
+        <v>1.2</v>
+      </c>
+      <c r="K41">
+        <v>0.84</v>
+      </c>
+      <c r="L41">
+        <v>17</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>5.6</v>
+      </c>
+      <c r="O41">
+        <v>1.7</v>
+      </c>
+      <c r="P41">
+        <v>1.2</v>
+      </c>
+      <c r="Q41">
+        <v>2.1</v>
+      </c>
+      <c r="R41">
+        <v>10</v>
+      </c>
+      <c r="S41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>27063613</v>
+      </c>
+      <c r="B42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42">
+        <v>607</v>
+      </c>
+      <c r="I42">
+        <v>0.80000001192092995</v>
+      </c>
+      <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
+        <v>0.91999998092652002</v>
+      </c>
+      <c r="L42">
+        <v>25</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>4</v>
+      </c>
+      <c r="O42">
+        <v>0.80000001192092995</v>
+      </c>
+      <c r="P42">
+        <v>2</v>
+      </c>
+      <c r="Q42">
+        <v>2.2999999523163002</v>
+      </c>
+      <c r="R42">
+        <v>12</v>
+      </c>
+      <c r="S42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43">
+        <v>698</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>0.8</v>
+      </c>
+      <c r="K43">
+        <v>0.76</v>
+      </c>
+      <c r="L43">
+        <v>22</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>8.4</v>
+      </c>
+      <c r="O43">
+        <v>2</v>
+      </c>
+      <c r="P43">
+        <v>0.8</v>
+      </c>
+      <c r="Q43">
+        <v>1.9</v>
+      </c>
+      <c r="R43">
+        <v>39</v>
+      </c>
+      <c r="S43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44">
+        <v>602</v>
+      </c>
+      <c r="I44">
+        <v>3.1</v>
+      </c>
+      <c r="J44">
+        <v>0.7</v>
+      </c>
+      <c r="K44">
+        <v>0.84</v>
+      </c>
+      <c r="L44">
+        <v>12</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="O44">
+        <v>3.1</v>
+      </c>
+      <c r="P44">
+        <v>0.7</v>
+      </c>
+      <c r="Q44">
+        <v>2.1</v>
+      </c>
+      <c r="R44">
+        <v>7</v>
+      </c>
+      <c r="S44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" t="s">
+        <v>52</v>
+      </c>
+      <c r="H45">
+        <v>827</v>
+      </c>
+      <c r="I45">
+        <v>4.5</v>
+      </c>
+      <c r="J45">
+        <v>1.5</v>
+      </c>
+      <c r="K45">
+        <v>0.72</v>
+      </c>
+      <c r="L45">
+        <v>14</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>15</v>
+      </c>
+      <c r="O45">
+        <v>4.5</v>
+      </c>
+      <c r="P45">
+        <v>1.5</v>
+      </c>
+      <c r="Q45">
+        <v>1.8</v>
+      </c>
+      <c r="R45">
+        <v>8</v>
+      </c>
+      <c r="S45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46">
+        <v>695</v>
+      </c>
+      <c r="I46">
+        <v>3.3</v>
+      </c>
+      <c r="J46">
+        <v>1.3</v>
+      </c>
+      <c r="K46">
+        <v>0.6</v>
+      </c>
+      <c r="L46">
+        <v>18.5</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>9.5</v>
+      </c>
+      <c r="O46">
+        <v>3.3</v>
+      </c>
+      <c r="P46">
+        <v>1.3</v>
+      </c>
+      <c r="Q46">
+        <v>1.5</v>
+      </c>
+      <c r="R46">
+        <v>9</v>
+      </c>
+      <c r="S46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>27007600</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47">
+        <v>4</v>
+      </c>
+      <c r="F47" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" t="s">
+        <v>62</v>
+      </c>
+      <c r="H47">
+        <v>1117</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>6.5</v>
+      </c>
+      <c r="K47">
+        <v>0.6</v>
+      </c>
+      <c r="L47">
+        <v>8.6000003814696999</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <v>22</v>
+      </c>
+      <c r="O47">
+        <v>2</v>
+      </c>
+      <c r="P47">
+        <v>6.5</v>
+      </c>
+      <c r="Q47">
+        <v>1.5</v>
+      </c>
+      <c r="R47">
+        <v>27</v>
+      </c>
+      <c r="S47" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48">
+        <v>343</v>
+      </c>
+      <c r="I48">
+        <v>0.1</v>
+      </c>
+      <c r="J48">
+        <v>3.1</v>
+      </c>
+      <c r="K48">
+        <v>1.4</v>
+      </c>
+      <c r="L48">
+        <v>16.8</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0.3</v>
+      </c>
+      <c r="O48">
+        <v>0.1</v>
+      </c>
+      <c r="P48">
+        <v>3.1</v>
+      </c>
+      <c r="Q48">
+        <v>3.5</v>
+      </c>
+      <c r="R48">
+        <v>9</v>
+      </c>
+      <c r="S48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" t="s">
+        <v>52</v>
+      </c>
+      <c r="H49">
+        <v>413</v>
+      </c>
+      <c r="I49">
+        <v>0.3</v>
+      </c>
+      <c r="J49">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K49">
+        <v>0.96</v>
+      </c>
+      <c r="L49">
+        <v>21</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>0.3</v>
+      </c>
+      <c r="P49">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q49">
+        <v>2.4</v>
+      </c>
+      <c r="R49">
+        <v>9</v>
+      </c>
+      <c r="S49" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout produit categroie C et E BD3
</commit_message>
<xml_diff>
--- a/Datasets/DB3.xlsx
+++ b/Datasets/DB3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USB 08.04.20\M2\S1\décision\projet\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamk\Desktop\Master\Transparance\projet-transparence\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB75A0C9-A41E-4327-812F-4E0BF02DB29C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DAC268-278B-421D-8E5D-8272752F85AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6EC24849-5032-4A96-8811-E4B54FE51E76}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="125">
   <si>
     <t>code</t>
   </si>
@@ -256,6 +256,159 @@
   </si>
   <si>
     <t>3560071011383</t>
+  </si>
+  <si>
+    <t>Blanc de poulet Halal - 4tr.</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Emincés de poulet rôti- 25% de sel*  - 2X75g</t>
+  </si>
+  <si>
+    <t>Nuggets au poulet bio</t>
+  </si>
+  <si>
+    <t>Boulettes De Volaille Bio</t>
+  </si>
+  <si>
+    <t>L'escalope Cordon Bleu de Poulet x4</t>
+  </si>
+  <si>
+    <t>Haché de poulet</t>
+  </si>
+  <si>
+    <t>Fines aiguillettes de Poulet Grillé</t>
+  </si>
+  <si>
+    <t>Manchons poulet crème oignon</t>
+  </si>
+  <si>
+    <t>Grignotte de poulet rôtie nature</t>
+  </si>
+  <si>
+    <t>Nuggets Extra Crosutillant x20</t>
+  </si>
+  <si>
+    <t>Frites de poulet panées</t>
+  </si>
+  <si>
+    <t>Nuggets de poulet aux pépites de fromage fondu</t>
+  </si>
+  <si>
+    <t>Ma Salade Duo</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Offals</t>
+  </si>
+  <si>
+    <t>Salami de poulet Halal</t>
+  </si>
+  <si>
+    <t>Magret de canard fumé prétranché</t>
+  </si>
+  <si>
+    <t>Le Magret de Canard du Sud-Ouest fumé au bois de hêtre</t>
+  </si>
+  <si>
+    <t>Magret canard fumé Labeyrie</t>
+  </si>
+  <si>
+    <t>Saucisse de filet de poulet fumées</t>
+  </si>
+  <si>
+    <t>Magret de Canard du Sud-Ouest Séché et au Poivre</t>
+  </si>
+  <si>
+    <t>Mousse de Canard au Porto</t>
+  </si>
+  <si>
+    <t>180G Confit Foie Volaille Grand Jury</t>
+  </si>
+  <si>
+    <t>4 saucisses de volaille façon charcutière aux herbes</t>
+  </si>
+  <si>
+    <t>Cuisses de canard gras confites MAISTRES OCCITANS, 4 pieces</t>
+  </si>
+  <si>
+    <t>Confit de canard du Sud Ouest au sel de Guerande BIRABEN, 2 cuisses</t>
+  </si>
+  <si>
+    <t>3266980674694</t>
+  </si>
+  <si>
+    <t>3760059785118</t>
+  </si>
+  <si>
+    <t>3067163623818</t>
+  </si>
+  <si>
+    <t>3515813232076</t>
+  </si>
+  <si>
+    <t>3033610061816</t>
+  </si>
+  <si>
+    <t>3237970000465</t>
+  </si>
+  <si>
+    <t>3564709019857</t>
+  </si>
+  <si>
+    <t>3256220271554</t>
+  </si>
+  <si>
+    <t>3245390201270</t>
+  </si>
+  <si>
+    <t>3230890017520</t>
+  </si>
+  <si>
+    <t>3292320040256</t>
+  </si>
+  <si>
+    <t>3443705008525</t>
+  </si>
+  <si>
+    <t>3095750507012</t>
+  </si>
+  <si>
+    <t>3095756221011</t>
+  </si>
+  <si>
+    <t>3266980677961</t>
+  </si>
+  <si>
+    <t>3095753025018</t>
+  </si>
+  <si>
+    <t>3760177214712</t>
+  </si>
+  <si>
+    <t>3564700756645</t>
+  </si>
+  <si>
+    <t>3256221654226</t>
+  </si>
+  <si>
+    <t>3266980266646</t>
+  </si>
+  <si>
+    <t>3266980134693</t>
+  </si>
+  <si>
+    <t>3230890744808</t>
+  </si>
+  <si>
+    <t>3422210440563</t>
+  </si>
+  <si>
+    <t>3422210436245</t>
   </si>
 </sst>
 </file>
@@ -608,15 +761,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B926D4-B8FA-4885-AAED-407EDDBDF88F}">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -1386,6 +1541,714 @@
         <v>32</v>
       </c>
     </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26">
+        <v>435</v>
+      </c>
+      <c r="I26">
+        <v>0.4</v>
+      </c>
+      <c r="J26">
+        <v>0.5</v>
+      </c>
+      <c r="K26">
+        <v>0.72</v>
+      </c>
+      <c r="L26">
+        <v>21</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>1.7</v>
+      </c>
+      <c r="O26">
+        <v>0.4</v>
+      </c>
+      <c r="P26">
+        <v>0.5</v>
+      </c>
+      <c r="Q26">
+        <v>1.8</v>
+      </c>
+      <c r="R26">
+        <v>69</v>
+      </c>
+      <c r="S26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27">
+        <v>698</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>0.8</v>
+      </c>
+      <c r="K27">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L27">
+        <v>22</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>8.4</v>
+      </c>
+      <c r="O27">
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <v>0.8</v>
+      </c>
+      <c r="Q27">
+        <v>1.4</v>
+      </c>
+      <c r="R27">
+        <v>66</v>
+      </c>
+      <c r="S27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28">
+        <v>1006</v>
+      </c>
+      <c r="I28">
+        <v>3.6</v>
+      </c>
+      <c r="J28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K28">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="L28">
+        <v>12.5</v>
+      </c>
+      <c r="M28">
+        <v>2.6</v>
+      </c>
+      <c r="N28">
+        <v>14</v>
+      </c>
+      <c r="O28">
+        <v>3.6</v>
+      </c>
+      <c r="P28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q28">
+        <v>1.38</v>
+      </c>
+      <c r="R28">
+        <v>48</v>
+      </c>
+      <c r="S28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29">
+        <v>690</v>
+      </c>
+      <c r="I29">
+        <v>2.4</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0.52</v>
+      </c>
+      <c r="L29">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>9</v>
+      </c>
+      <c r="O29">
+        <v>2.4</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>1.3</v>
+      </c>
+      <c r="R29">
+        <v>66</v>
+      </c>
+      <c r="S29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30">
+        <v>481</v>
+      </c>
+      <c r="I30">
+        <v>0.4</v>
+      </c>
+      <c r="J30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K30">
+        <v>0.72</v>
+      </c>
+      <c r="L30">
+        <v>22</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <v>1.7</v>
+      </c>
+      <c r="O30">
+        <v>0.4</v>
+      </c>
+      <c r="P30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q30">
+        <v>1.8</v>
+      </c>
+      <c r="R30">
+        <v>69</v>
+      </c>
+      <c r="S30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31">
+        <v>857</v>
+      </c>
+      <c r="I31">
+        <v>3.6</v>
+      </c>
+      <c r="J31">
+        <v>0.7</v>
+      </c>
+      <c r="K31">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L31">
+        <v>23</v>
+      </c>
+      <c r="M31">
+        <v>1.2</v>
+      </c>
+      <c r="N31">
+        <v>12</v>
+      </c>
+      <c r="O31">
+        <v>3.6</v>
+      </c>
+      <c r="P31">
+        <v>0.7</v>
+      </c>
+      <c r="Q31">
+        <v>1.4</v>
+      </c>
+      <c r="R31">
+        <v>48</v>
+      </c>
+      <c r="S31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32">
+        <v>803</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>0.44</v>
+      </c>
+      <c r="L32">
+        <v>22</v>
+      </c>
+      <c r="M32">
+        <v>0.5</v>
+      </c>
+      <c r="N32">
+        <v>11</v>
+      </c>
+      <c r="O32">
+        <v>3</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R32">
+        <v>63</v>
+      </c>
+      <c r="S32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33">
+        <v>892</v>
+      </c>
+      <c r="I33">
+        <v>2.5</v>
+      </c>
+      <c r="J33">
+        <v>1.2</v>
+      </c>
+      <c r="K33">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="L33">
+        <v>11.9</v>
+      </c>
+      <c r="M33">
+        <v>1.7</v>
+      </c>
+      <c r="N33">
+        <v>11</v>
+      </c>
+      <c r="O33">
+        <v>2.5</v>
+      </c>
+      <c r="P33">
+        <v>1.2</v>
+      </c>
+      <c r="Q33">
+        <v>1.44</v>
+      </c>
+      <c r="R33">
+        <v>75</v>
+      </c>
+      <c r="S33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34">
+        <v>1047</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34">
+        <v>1.9</v>
+      </c>
+      <c r="K34">
+        <v>0.44</v>
+      </c>
+      <c r="L34">
+        <v>13</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>15</v>
+      </c>
+      <c r="O34">
+        <v>3</v>
+      </c>
+      <c r="P34">
+        <v>1.9</v>
+      </c>
+      <c r="Q34">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R34">
+        <v>54</v>
+      </c>
+      <c r="S34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35">
+        <v>1015</v>
+      </c>
+      <c r="I35">
+        <v>2.5</v>
+      </c>
+      <c r="J35">
+        <v>1.6</v>
+      </c>
+      <c r="K35">
+        <v>0.48</v>
+      </c>
+      <c r="L35">
+        <v>13</v>
+      </c>
+      <c r="M35">
+        <v>1.3</v>
+      </c>
+      <c r="N35">
+        <v>12</v>
+      </c>
+      <c r="O35">
+        <v>2.5</v>
+      </c>
+      <c r="P35">
+        <v>1.6</v>
+      </c>
+      <c r="Q35">
+        <v>1.2</v>
+      </c>
+      <c r="R35">
+        <v>42</v>
+      </c>
+      <c r="S35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36">
+        <v>979</v>
+      </c>
+      <c r="I36">
+        <v>3.4</v>
+      </c>
+      <c r="J36">
+        <v>2.5</v>
+      </c>
+      <c r="K36">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="L36">
+        <v>16</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>16.59</v>
+      </c>
+      <c r="O36">
+        <v>3.4</v>
+      </c>
+      <c r="P36">
+        <v>2.5</v>
+      </c>
+      <c r="Q36">
+        <v>1.33</v>
+      </c>
+      <c r="R36">
+        <v>73</v>
+      </c>
+      <c r="S36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37">
+        <v>992</v>
+      </c>
+      <c r="I37">
+        <v>1.6</v>
+      </c>
+      <c r="J37">
+        <v>0.9</v>
+      </c>
+      <c r="K37">
+        <v>0.48</v>
+      </c>
+      <c r="L37">
+        <v>13</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>11</v>
+      </c>
+      <c r="O37">
+        <v>1.6</v>
+      </c>
+      <c r="P37">
+        <v>0.9</v>
+      </c>
+      <c r="Q37">
+        <v>1.2</v>
+      </c>
+      <c r="R37">
+        <v>79</v>
+      </c>
+      <c r="S37" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>50</v>
@@ -2091,6 +2954,714 @@
         <v>9</v>
       </c>
       <c r="S49" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>88</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" t="s">
+        <v>89</v>
+      </c>
+      <c r="H50">
+        <v>1151</v>
+      </c>
+      <c r="I50">
+        <v>6.5</v>
+      </c>
+      <c r="J50">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K50">
+        <v>1.2</v>
+      </c>
+      <c r="L50">
+        <v>22</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>20</v>
+      </c>
+      <c r="O50">
+        <v>6.5</v>
+      </c>
+      <c r="P50">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q50">
+        <v>3</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E51">
+        <v>4</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51">
+        <v>1467</v>
+      </c>
+      <c r="I51">
+        <v>15</v>
+      </c>
+      <c r="J51">
+        <v>0.5</v>
+      </c>
+      <c r="K51">
+        <v>1.6</v>
+      </c>
+      <c r="L51">
+        <v>20</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>30</v>
+      </c>
+      <c r="O51">
+        <v>15</v>
+      </c>
+      <c r="P51">
+        <v>0.5</v>
+      </c>
+      <c r="Q51">
+        <v>4</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
+      </c>
+      <c r="S51" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52">
+        <v>3</v>
+      </c>
+      <c r="F52" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52">
+        <v>1460</v>
+      </c>
+      <c r="I52">
+        <v>11</v>
+      </c>
+      <c r="J52">
+        <v>0.6</v>
+      </c>
+      <c r="K52">
+        <v>1.48</v>
+      </c>
+      <c r="L52">
+        <v>20</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>30</v>
+      </c>
+      <c r="O52">
+        <v>11</v>
+      </c>
+      <c r="P52">
+        <v>0.6</v>
+      </c>
+      <c r="Q52">
+        <v>3.7</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>88</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+      <c r="F53" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" t="s">
+        <v>26</v>
+      </c>
+      <c r="H53">
+        <v>1424</v>
+      </c>
+      <c r="I53">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J53">
+        <v>0.5</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>19</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>28</v>
+      </c>
+      <c r="O53">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="P53">
+        <v>0.5</v>
+      </c>
+      <c r="Q53">
+        <v>2.5</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54">
+        <v>1349</v>
+      </c>
+      <c r="I54">
+        <v>10</v>
+      </c>
+      <c r="J54">
+        <v>0.7</v>
+      </c>
+      <c r="K54">
+        <v>1.08</v>
+      </c>
+      <c r="L54">
+        <v>19</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>27</v>
+      </c>
+      <c r="O54">
+        <v>10</v>
+      </c>
+      <c r="P54">
+        <v>0.7</v>
+      </c>
+      <c r="Q54">
+        <v>2.7</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>88</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H55">
+        <v>937</v>
+      </c>
+      <c r="I55">
+        <v>10</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="L55">
+        <v>20</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>15.49</v>
+      </c>
+      <c r="O55">
+        <v>10</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>88</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" t="s">
+        <v>26</v>
+      </c>
+      <c r="H56">
+        <v>1711</v>
+      </c>
+      <c r="I56">
+        <v>12</v>
+      </c>
+      <c r="J56">
+        <v>0.3</v>
+      </c>
+      <c r="K56">
+        <v>1.32</v>
+      </c>
+      <c r="L56">
+        <v>22</v>
+      </c>
+      <c r="M56">
+        <v>0.5</v>
+      </c>
+      <c r="N56">
+        <v>36</v>
+      </c>
+      <c r="O56">
+        <v>12</v>
+      </c>
+      <c r="P56">
+        <v>0.3</v>
+      </c>
+      <c r="Q56">
+        <v>3.3</v>
+      </c>
+      <c r="R56">
+        <v>30</v>
+      </c>
+      <c r="S56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57">
+        <v>4</v>
+      </c>
+      <c r="F57" t="s">
+        <v>61</v>
+      </c>
+      <c r="G57" t="s">
+        <v>62</v>
+      </c>
+      <c r="H57">
+        <v>1587</v>
+      </c>
+      <c r="I57">
+        <v>14</v>
+      </c>
+      <c r="J57">
+        <v>1.3</v>
+      </c>
+      <c r="K57">
+        <v>0.64</v>
+      </c>
+      <c r="L57">
+        <v>10</v>
+      </c>
+      <c r="M57">
+        <v>0.5</v>
+      </c>
+      <c r="N57">
+        <v>37</v>
+      </c>
+      <c r="O57">
+        <v>14</v>
+      </c>
+      <c r="P57">
+        <v>1.3</v>
+      </c>
+      <c r="Q57">
+        <v>1.6</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58">
+        <v>4</v>
+      </c>
+      <c r="F58" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" t="s">
+        <v>62</v>
+      </c>
+      <c r="H58">
+        <v>1272</v>
+      </c>
+      <c r="I58">
+        <v>11</v>
+      </c>
+      <c r="J58">
+        <v>0.5</v>
+      </c>
+      <c r="K58">
+        <v>0.6</v>
+      </c>
+      <c r="L58">
+        <v>13.5</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>27.5</v>
+      </c>
+      <c r="O58">
+        <v>11</v>
+      </c>
+      <c r="P58">
+        <v>0.5</v>
+      </c>
+      <c r="Q58">
+        <v>1.5</v>
+      </c>
+      <c r="R58">
+        <v>24</v>
+      </c>
+      <c r="S58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" t="s">
+        <v>52</v>
+      </c>
+      <c r="H59">
+        <v>1248</v>
+      </c>
+      <c r="I59">
+        <v>11</v>
+      </c>
+      <c r="J59">
+        <v>0.8</v>
+      </c>
+      <c r="K59">
+        <v>0.6</v>
+      </c>
+      <c r="L59">
+        <v>16</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>26</v>
+      </c>
+      <c r="O59">
+        <v>11</v>
+      </c>
+      <c r="P59">
+        <v>0.8</v>
+      </c>
+      <c r="Q59">
+        <v>1.5</v>
+      </c>
+      <c r="R59">
+        <v>30</v>
+      </c>
+      <c r="S59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+      <c r="F60" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60">
+        <v>1351</v>
+      </c>
+      <c r="I60">
+        <v>8.1</v>
+      </c>
+      <c r="J60">
+        <v>0.5</v>
+      </c>
+      <c r="K60">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="L60">
+        <v>24</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>24</v>
+      </c>
+      <c r="O60">
+        <v>8.1</v>
+      </c>
+      <c r="P60">
+        <v>0.5</v>
+      </c>
+      <c r="Q60">
+        <v>2.04</v>
+      </c>
+      <c r="R60">
+        <v>30</v>
+      </c>
+      <c r="S60" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61">
+        <v>1519</v>
+      </c>
+      <c r="I61">
+        <v>10</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>0.64</v>
+      </c>
+      <c r="L61">
+        <v>22</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>31</v>
+      </c>
+      <c r="O61">
+        <v>10</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>1.6</v>
+      </c>
+      <c r="R61">
+        <v>30</v>
+      </c>
+      <c r="S61" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>